<commit_message>
2024_03_09_14_52 Updated Stock Analysis Files
</commit_message>
<xml_diff>
--- a/02_data/stock_term_descriptions.xlsx
+++ b/02_data/stock_term_descriptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Dropbox\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="124" documentId="13_ncr:1_{AF29CE8C-0FBE-4720-B983-9BAE9B572625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B3ADEF1-D6F8-41E0-8619-B97FB7812270}"/>
+  <xr:revisionPtr revIDLastSave="129" documentId="13_ncr:1_{AF29CE8C-0FBE-4720-B983-9BAE9B572625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3BBFDCD-BF29-4BD7-B34F-0C637C77C04E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DDA6B01A-A375-4C0C-A424-0FCF9D2D055F}"/>
   </bookViews>
@@ -39,15 +39,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="166">
-  <si>
-    <t>Include</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="167">
+  <si>
+    <t>include</t>
   </si>
   <si>
     <t>stock_attributes</t>
   </si>
   <si>
-    <t>Descriptions</t>
+    <t>descriptions</t>
   </si>
   <si>
     <t>52WeekChange</t>
@@ -414,6 +414,9 @@
   </si>
   <si>
     <t>regularMarketOpen</t>
+  </si>
+  <si>
+    <t>The regular market trades from 9:30 a.m. to 4 p.m. ET</t>
   </si>
   <si>
     <t>regularMarketPreviousClose</t>
@@ -921,7 +924,7 @@
   <dimension ref="A1:D107"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1436,222 +1439,225 @@
         <v>121</v>
       </c>
     </row>
-    <row r="65" spans="2:2">
+    <row r="65" spans="2:3">
       <c r="B65" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="66" spans="2:2">
+    <row r="66" spans="2:3">
       <c r="B66" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="67" spans="2:2">
+    <row r="67" spans="2:3">
       <c r="B67" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="68" spans="2:2">
+      <c r="C67" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3">
       <c r="B68" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="69" spans="2:2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3">
       <c r="B69" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="70" spans="2:2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3">
       <c r="B70" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="71" spans="2:2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3">
       <c r="B71" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="72" spans="2:2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3">
       <c r="B72" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="73" spans="2:2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3">
       <c r="B73" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="74" spans="2:2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3">
       <c r="B74" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="75" spans="2:2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3">
       <c r="B75" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="76" spans="2:2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3">
       <c r="B76" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="77" spans="2:2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3">
       <c r="B77" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="78" spans="2:2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3">
       <c r="B78" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="79" spans="2:2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3">
       <c r="B79" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="80" spans="2:2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3">
       <c r="B80" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="81" spans="2:3">
       <c r="B81" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="82" spans="2:3">
       <c r="B82" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="83" spans="2:3">
       <c r="B83" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="84" spans="2:3">
       <c r="B84" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="85" spans="2:3">
       <c r="B85" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="86" spans="2:3">
       <c r="B86" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C86" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="87" spans="2:3">
       <c r="B87" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="88" spans="2:3">
       <c r="B88" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="89" spans="2:3">
       <c r="B89" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="90" spans="2:3">
       <c r="B90" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="91" spans="2:3">
       <c r="B91" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="92" spans="2:3">
       <c r="B92" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="93" spans="2:3">
       <c r="B93" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="94" spans="2:3">
       <c r="B94" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="95" spans="2:3">
       <c r="B95" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="96" spans="2:3">
       <c r="B96" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="97" spans="2:2">
       <c r="B97" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="98" spans="2:2">
       <c r="B98" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="99" spans="2:2">
       <c r="B99" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="100" spans="2:2">
       <c r="B100" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="101" spans="2:2">
       <c r="B101" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="102" spans="2:2">
       <c r="B102" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="103" spans="2:2">
       <c r="B103" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="104" spans="2:2">
       <c r="B104" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="105" spans="2:2">
       <c r="B105" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="106" spans="2:2">
       <c r="B106" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="107" spans="2:2">
       <c r="B107" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2024_03_09_14_53 Updated Stock Analysis Files
</commit_message>
<xml_diff>
--- a/02_data/stock_term_descriptions.xlsx
+++ b/02_data/stock_term_descriptions.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Dropbox\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="129" documentId="13_ncr:1_{AF29CE8C-0FBE-4720-B983-9BAE9B572625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3BBFDCD-BF29-4BD7-B34F-0C637C77C04E}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="13_ncr:1_{AF29CE8C-0FBE-4720-B983-9BAE9B572625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A782C0E9-E30B-47A7-95F9-7D034D1E6FE6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DDA6B01A-A375-4C0C-A424-0FCF9D2D055F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="stock_attributes" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$C$107</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">stock_attributes!$B$1:$C$107</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -416,10 +416,10 @@
     <t>regularMarketOpen</t>
   </si>
   <si>
-    <t>The regular market trades from 9:30 a.m. to 4 p.m. ET</t>
-  </si>
-  <si>
     <t>regularMarketPreviousClose</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Previous close is a security's closing price on the preceding time period of the one being referenced. Previous close almost always refers to the prior day's final price of a security when the market officially closes for the day.</t>
   </si>
   <si>
     <t>regularMarketVolume</t>
@@ -923,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49198A2D-A825-4E1E-8E0A-42488D51E54F}">
   <dimension ref="A1:D107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="B48" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1453,12 +1453,12 @@
       <c r="B67" t="s">
         <v>124</v>
       </c>
-      <c r="C67" t="s">
-        <v>125</v>
-      </c>
     </row>
     <row r="68" spans="2:3">
       <c r="B68" t="s">
+        <v>125</v>
+      </c>
+      <c r="C68" t="s">
         <v>126</v>
       </c>
     </row>

</xml_diff>